<commit_message>
add BP (batas penggunaan) to data structure and data generation
</commit_message>
<xml_diff>
--- a/test/testdata4.xlsx
+++ b/test/testdata4.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Bank Indonesia Pematang Siantar</t>
   </si>
   <si>
-    <t xml:space="preserve">freq</t>
+    <t xml:space="preserve">BP</t>
   </si>
   <si>
     <t xml:space="preserve">cover</t>
@@ -139,13 +139,10 @@
     <t xml:space="preserve">truck</t>
   </si>
   <si>
+    <t xml:space="preserve">3 0 0 0 0</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 2 3 4 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">truck B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2 3 4</t>
   </si>
   <si>
     <t xml:space="preserve">T</t>
@@ -413,7 +410,7 @@
     <tableColumn id="1" name="id"/>
     <tableColumn id="2" name="name"/>
     <tableColumn id="3" name="type"/>
-    <tableColumn id="4" name="freq"/>
+    <tableColumn id="4" name="BP"/>
     <tableColumn id="5" name="cover"/>
     <tableColumn id="6" name="CON"/>
     <tableColumn id="7" name="Q (CT)"/>
@@ -472,11 +469,11 @@
   </sheetPr>
   <dimension ref="A1:N1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.42"/>
@@ -1019,18 +1016,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.48"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="6" min="6" style="0" width="7.29"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="7" min="7" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="5.01"/>
@@ -1113,11 +1110,11 @@
       <c r="C2" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>2</v>
+      <c r="D2" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1000</v>
@@ -1162,42 +1159,16 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>3000</v>
-      </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
-      <c r="K3" s="7" t="n">
-        <v>0</v>
-      </c>
+      <c r="K3" s="7"/>
       <c r="L3" s="7"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="7" t="n">
-        <v>0</v>
-      </c>
+      <c r="N3" s="7"/>
       <c r="O3" s="6"/>
-      <c r="P3" s="7" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="P3" s="7"/>
       <c r="Q3" s="6"/>
-      <c r="R3" s="7" t="n">
-        <v>1</v>
-      </c>
+      <c r="R3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I4" s="6"/>
@@ -1908,12 +1879,19 @@
       <c r="R62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I63" s="6"/>
-      <c r="J63" s="6"/>
-      <c r="K63" s="7"/>
-      <c r="L63" s="7"/>
-      <c r="M63" s="6"/>
-      <c r="N63" s="7"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="10"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="10"/>
       <c r="O63" s="6"/>
       <c r="P63" s="7"/>
       <c r="Q63" s="6"/>
@@ -2053,9 +2031,9 @@
       <c r="R70" s="7"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="8"/>
+      <c r="B71" s="11"/>
       <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
+      <c r="D71" s="11"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -2072,9 +2050,9 @@
       <c r="R71" s="7"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="11"/>
+      <c r="B72" s="8"/>
       <c r="C72" s="8"/>
-      <c r="D72" s="11"/>
+      <c r="D72" s="8"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -2243,19 +2221,12 @@
       <c r="R80" s="7"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="8"/>
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="10"/>
-      <c r="L81" s="10"/>
-      <c r="M81" s="9"/>
-      <c r="N81" s="10"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="6"/>
+      <c r="N81" s="7"/>
       <c r="O81" s="6"/>
       <c r="P81" s="7"/>
       <c r="Q81" s="6"/>
@@ -2285,18 +2256,7 @@
       <c r="Q83" s="6"/>
       <c r="R83" s="7"/>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I84" s="6"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="7"/>
-      <c r="L84" s="7"/>
-      <c r="M84" s="6"/>
-      <c r="N84" s="7"/>
-      <c r="O84" s="6"/>
-      <c r="P84" s="7"/>
-      <c r="Q84" s="6"/>
-      <c r="R84" s="7"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2318,18 +2278,18 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2361,11 +2321,11 @@
   </sheetPr>
   <dimension ref="A1:Q147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.13"/>

</xml_diff>